<commit_message>
comit last 23 1 2019
</commit_message>
<xml_diff>
--- a/Tamplo5/src/main/java/com/tamplo/qa/testdata/autoationtestdata.xlsx
+++ b/Tamplo5/src/main/java/com/tamplo/qa/testdata/autoationtestdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="3570"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>login name</t>
+    <t>username</t>
   </si>
   <si>
     <t>password</t>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>nitin.tajane@yahoo.com</t>
-  </si>
-  <si>
-    <t>nitin.tajane@yandex.com</t>
   </si>
 </sst>
 </file>
@@ -363,23 +360,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -396,14 +392,6 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
         <v>1234</v>
       </c>
     </row>
@@ -419,7 +407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -431,7 +419,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>